<commit_message>
Updated metadata files, qsub scripts and the bbmerge settings.
</commit_message>
<xml_diff>
--- a/data/metadata_final.xlsx
+++ b/data/metadata_final.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="580" windowWidth="42380" windowHeight="25240" tabRatio="500"/>
+    <workbookView xWindow="3360" yWindow="20" windowWidth="42380" windowHeight="25240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,48 +591,6 @@
     <t>BH73_94_3.fq.gz</t>
   </si>
   <si>
-    <t>4c4a4e8054976969e0a3e5cfbebc7996f5a6bccf</t>
-  </si>
-  <si>
-    <t>08f05ccca1f14aaca1ca9ff28c39f6e09d37ef58</t>
-  </si>
-  <si>
-    <t>b9e61def20d1ed2e7c4123dbd691e172b756214d</t>
-  </si>
-  <si>
-    <t>d5e33fb713c6999c25c9949233401ed0e238ab50</t>
-  </si>
-  <si>
-    <t>ef0f053e9da7d0f25ceca4b7c057074b5dc9a4aa</t>
-  </si>
-  <si>
-    <t>007b464571c166cbfdf8a7f7f984ea11962f7d17</t>
-  </si>
-  <si>
-    <t>84a9dce8b9ee8c2f3205129993fcc60ae0a75363</t>
-  </si>
-  <si>
-    <t>79756c1c780b438dcc6ec4d0b43e3a91a1d8bc9a</t>
-  </si>
-  <si>
-    <t>39c9116c6f433015c38977b62f893fd3d6adc9e4</t>
-  </si>
-  <si>
-    <t>ba940c393c5786a0bed303c667ca38f22589f94d</t>
-  </si>
-  <si>
-    <t>c194d8467f7fbe0041d8a99b51acda2d1439ab02</t>
-  </si>
-  <si>
-    <t>de49f158de10126a958897b411f8589eec84ebf7</t>
-  </si>
-  <si>
-    <t>0c8dcda3bd406f5c470324253b6184ab7b562859</t>
-  </si>
-  <si>
-    <t>467a495a5c1cdab9660e6e90af70fe3c9ba0e0da</t>
-  </si>
-  <si>
     <t>b40e661ab39cbbaeafd0c54a767b1141ed5078c6</t>
   </si>
   <si>
@@ -832,6 +790,48 @@
   </si>
   <si>
     <t>Reverse</t>
+  </si>
+  <si>
+    <t>14bafc7debe4ad7be2650046d762fc47f6a6fa3d</t>
+  </si>
+  <si>
+    <t>a476c19a529b832d953ce11c4e6bb66bf013cc5d</t>
+  </si>
+  <si>
+    <t>27ed9bf6dc1fdb6846a6c71915236d2fc3c79e0a</t>
+  </si>
+  <si>
+    <t>33d1be909d9d868feb00019bdbd9a39baace4f85</t>
+  </si>
+  <si>
+    <t>942d9d138cc9a390885e1a4b1f6277aaff786c32</t>
+  </si>
+  <si>
+    <t>20ce561c626cffc45e90731f4087c600ff4bd804</t>
+  </si>
+  <si>
+    <t>9b0ab37a9f649fbc288194835870317ae3d2c430</t>
+  </si>
+  <si>
+    <t>37deb28a323983fa7845f27179276938b7500935</t>
+  </si>
+  <si>
+    <t>168650418db6e9e2bb542d56ba0524fd9f535d0b</t>
+  </si>
+  <si>
+    <t>4a5d93914924dce39f6e12aacd1b686eb37323db</t>
+  </si>
+  <si>
+    <t>65875071cdd9455baed876333727edef78467065</t>
+  </si>
+  <si>
+    <t>84e804b9abb637994a4fb18213c6f64d4dd3c431</t>
+  </si>
+  <si>
+    <t>a4106a6f02dd6370b4d878c1f75edb6c590b1db4</t>
+  </si>
+  <si>
+    <t>3d21556ad4f619f9f77f96c4cfd76d0c10367b1f</t>
   </si>
 </sst>
 </file>
@@ -892,8 +892,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1037,7 +1043,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1102,6 +1108,9 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1166,6 +1175,9 @@
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1497,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28:Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1529,10 +1541,10 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="D1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1547,10 +1559,10 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J1" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -1565,13 +1577,13 @@
         <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="P1" t="s">
         <v>4</v>
       </c>
       <c r="Q1" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1602,7 +1614,7 @@
         <v>1683</v>
       </c>
       <c r="I2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
@@ -1620,13 +1632,13 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P2">
         <v>100</v>
       </c>
       <c r="Q2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1657,7 +1669,7 @@
         <v>1806</v>
       </c>
       <c r="I3" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
@@ -1675,13 +1687,13 @@
         <v>6</v>
       </c>
       <c r="O3" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P3">
         <v>100</v>
       </c>
       <c r="Q3" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1712,7 +1724,7 @@
         <v>1801</v>
       </c>
       <c r="I4" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
@@ -1730,13 +1742,13 @@
         <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P4">
         <v>100</v>
       </c>
       <c r="Q4" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1767,7 +1779,7 @@
         <v>1794</v>
       </c>
       <c r="I5" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
@@ -1785,13 +1797,13 @@
         <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P5">
         <v>100</v>
       </c>
       <c r="Q5" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1822,7 +1834,7 @@
         <v>1789</v>
       </c>
       <c r="I6" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
@@ -1840,13 +1852,13 @@
         <v>6</v>
       </c>
       <c r="O6" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P6">
         <v>100</v>
       </c>
       <c r="Q6" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1877,7 +1889,7 @@
         <v>1789</v>
       </c>
       <c r="I7" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
@@ -1895,13 +1907,13 @@
         <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P7">
         <v>100</v>
       </c>
       <c r="Q7" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1932,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
@@ -1950,13 +1962,13 @@
         <v>6</v>
       </c>
       <c r="O8" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P8">
         <v>100</v>
       </c>
       <c r="Q8" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1987,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
@@ -2005,13 +2017,13 @@
         <v>6</v>
       </c>
       <c r="O9" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P9">
         <v>100</v>
       </c>
       <c r="Q9" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2042,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J10" t="s">
         <v>6</v>
@@ -2060,13 +2072,13 @@
         <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P10">
         <v>100</v>
       </c>
       <c r="Q10" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2097,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J11" t="s">
         <v>6</v>
@@ -2115,13 +2127,13 @@
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P11">
         <v>100</v>
       </c>
       <c r="Q11" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2152,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J12" t="s">
         <v>6</v>
@@ -2170,13 +2182,13 @@
         <v>6</v>
       </c>
       <c r="O12" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P12">
         <v>100</v>
       </c>
       <c r="Q12" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2207,7 +2219,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
@@ -2225,13 +2237,13 @@
         <v>6</v>
       </c>
       <c r="O13" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P13">
         <v>100</v>
       </c>
       <c r="Q13" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2262,7 +2274,7 @@
         <v>1709</v>
       </c>
       <c r="I14" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
@@ -2280,13 +2292,13 @@
         <v>6</v>
       </c>
       <c r="O14" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P14">
         <v>100</v>
       </c>
       <c r="Q14" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2317,7 +2329,7 @@
         <v>1704</v>
       </c>
       <c r="I15" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J15" t="s">
         <v>6</v>
@@ -2335,13 +2347,13 @@
         <v>6</v>
       </c>
       <c r="O15" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P15">
         <v>100</v>
       </c>
       <c r="Q15" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2372,7 +2384,7 @@
         <v>1898</v>
       </c>
       <c r="I16" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J16" t="s">
         <v>6</v>
@@ -2390,13 +2402,13 @@
         <v>6</v>
       </c>
       <c r="O16" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P16">
         <v>100</v>
       </c>
       <c r="Q16" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2427,7 +2439,7 @@
         <v>1887</v>
       </c>
       <c r="I17" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J17" t="s">
         <v>6</v>
@@ -2445,13 +2457,13 @@
         <v>6</v>
       </c>
       <c r="O17" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P17">
         <v>100</v>
       </c>
       <c r="Q17" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2482,7 +2494,7 @@
         <v>1964</v>
       </c>
       <c r="I18" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J18" t="s">
         <v>6</v>
@@ -2500,13 +2512,13 @@
         <v>6</v>
       </c>
       <c r="O18" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P18">
         <v>100</v>
       </c>
       <c r="Q18" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2537,7 +2549,7 @@
         <v>1866</v>
       </c>
       <c r="I19" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J19" t="s">
         <v>6</v>
@@ -2555,13 +2567,13 @@
         <v>6</v>
       </c>
       <c r="O19" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P19">
         <v>100</v>
       </c>
       <c r="Q19" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2592,7 +2604,7 @@
         <v>1863</v>
       </c>
       <c r="I20" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J20" t="s">
         <v>6</v>
@@ -2610,13 +2622,13 @@
         <v>6</v>
       </c>
       <c r="O20" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P20">
         <v>100</v>
       </c>
       <c r="Q20" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2647,7 +2659,7 @@
         <v>1860</v>
       </c>
       <c r="I21" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J21" t="s">
         <v>6</v>
@@ -2665,13 +2677,13 @@
         <v>6</v>
       </c>
       <c r="O21" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P21">
         <v>100</v>
       </c>
       <c r="Q21" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2702,7 +2714,7 @@
         <v>1788</v>
       </c>
       <c r="I22" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J22" t="s">
         <v>6</v>
@@ -2720,13 +2732,13 @@
         <v>6</v>
       </c>
       <c r="O22" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P22">
         <v>100</v>
       </c>
       <c r="Q22" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2757,7 +2769,7 @@
         <v>1786</v>
       </c>
       <c r="I23" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J23" t="s">
         <v>6</v>
@@ -2775,13 +2787,13 @@
         <v>6</v>
       </c>
       <c r="O23" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P23">
         <v>100</v>
       </c>
       <c r="Q23" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2812,7 +2824,7 @@
         <v>1766</v>
       </c>
       <c r="I24" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J24" t="s">
         <v>6</v>
@@ -2830,13 +2842,13 @@
         <v>6</v>
       </c>
       <c r="O24" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P24">
         <v>100</v>
       </c>
       <c r="Q24" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2867,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J25" t="s">
         <v>6</v>
@@ -2885,13 +2897,13 @@
         <v>6</v>
       </c>
       <c r="O25" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P25">
         <v>100</v>
       </c>
       <c r="Q25" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2922,7 +2934,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J26" t="s">
         <v>6</v>
@@ -2940,13 +2952,13 @@
         <v>6</v>
       </c>
       <c r="O26" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P26">
         <v>100</v>
       </c>
       <c r="Q26" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2977,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J27" t="s">
         <v>6</v>
@@ -2995,13 +3007,13 @@
         <v>6</v>
       </c>
       <c r="O27" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="P27">
         <v>100</v>
       </c>
       <c r="Q27" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -3032,10 +3044,10 @@
         <v>1716</v>
       </c>
       <c r="I28" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J28" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K28" t="s">
         <v>62</v>
@@ -3050,13 +3062,13 @@
         <v>101</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P28">
         <v>100</v>
       </c>
       <c r="Q28" t="s">
-        <v>189</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -3087,10 +3099,10 @@
         <v>1714</v>
       </c>
       <c r="I29" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J29" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K29" t="s">
         <v>62</v>
@@ -3105,13 +3117,13 @@
         <v>101</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P29">
         <v>100</v>
       </c>
       <c r="Q29" t="s">
-        <v>190</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -3142,10 +3154,10 @@
         <v>1935</v>
       </c>
       <c r="I30" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J30" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K30" t="s">
         <v>62</v>
@@ -3160,13 +3172,13 @@
         <v>101</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P30">
         <v>100</v>
       </c>
       <c r="Q30" t="s">
-        <v>191</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -3197,10 +3209,10 @@
         <v>1920</v>
       </c>
       <c r="I31" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J31" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K31" t="s">
         <v>62</v>
@@ -3215,13 +3227,13 @@
         <v>101</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P31">
         <v>100</v>
       </c>
       <c r="Q31" t="s">
-        <v>192</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -3252,10 +3264,10 @@
         <v>1875</v>
       </c>
       <c r="I32" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J32" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K32" t="s">
         <v>62</v>
@@ -3270,13 +3282,13 @@
         <v>101</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P32">
         <v>100</v>
       </c>
       <c r="Q32" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -3307,10 +3319,10 @@
         <v>1874</v>
       </c>
       <c r="I33" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J33" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K33" t="s">
         <v>62</v>
@@ -3325,13 +3337,13 @@
         <v>101</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P33">
         <v>100</v>
       </c>
       <c r="Q33" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -3362,10 +3374,10 @@
         <v>1873</v>
       </c>
       <c r="I34" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J34" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K34" t="s">
         <v>62</v>
@@ -3380,13 +3392,13 @@
         <v>101</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P34">
         <v>100</v>
       </c>
       <c r="Q34" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -3417,10 +3429,10 @@
         <v>1871</v>
       </c>
       <c r="I35" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J35" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K35" t="s">
         <v>62</v>
@@ -3435,13 +3447,13 @@
         <v>101</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P35">
         <v>100</v>
       </c>
       <c r="Q35" t="s">
-        <v>196</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -3472,10 +3484,10 @@
         <v>1869</v>
       </c>
       <c r="I36" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J36" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K36" t="s">
         <v>62</v>
@@ -3490,13 +3502,13 @@
         <v>101</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P36">
         <v>100</v>
       </c>
       <c r="Q36" t="s">
-        <v>197</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -3527,10 +3539,10 @@
         <v>1857</v>
       </c>
       <c r="I37" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J37" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>11</v>
@@ -3545,13 +3557,13 @@
         <v>101</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P37">
         <v>100</v>
       </c>
       <c r="Q37" t="s">
-        <v>198</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3582,10 +3594,10 @@
         <v>1854</v>
       </c>
       <c r="I38" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J38" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K38" t="s">
         <v>62</v>
@@ -3600,13 +3612,13 @@
         <v>101</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P38">
         <v>100</v>
       </c>
       <c r="Q38" t="s">
-        <v>199</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -3637,10 +3649,10 @@
         <v>1850</v>
       </c>
       <c r="I39" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J39" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K39" t="s">
         <v>62</v>
@@ -3655,13 +3667,13 @@
         <v>101</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P39">
         <v>100</v>
       </c>
-      <c r="Q39" t="s">
-        <v>200</v>
+      <c r="Q39" s="9" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -3692,10 +3704,10 @@
         <v>1843</v>
       </c>
       <c r="I40" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J40" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K40" t="s">
         <v>62</v>
@@ -3710,13 +3722,13 @@
         <v>101</v>
       </c>
       <c r="O40" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="P40">
+        <v>100</v>
+      </c>
+      <c r="Q40" t="s">
         <v>268</v>
-      </c>
-      <c r="P40">
-        <v>100</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3747,10 +3759,10 @@
         <v>1837</v>
       </c>
       <c r="I41" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J41" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K41" t="s">
         <v>62</v>
@@ -3765,13 +3777,13 @@
         <v>101</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P41">
         <v>100</v>
       </c>
       <c r="Q41" t="s">
-        <v>202</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -3802,10 +3814,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J42" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K42" t="s">
         <v>62</v>
@@ -3820,13 +3832,13 @@
         <v>101</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P42">
         <v>100</v>
       </c>
       <c r="Q42" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3857,10 +3869,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J43" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K43" t="s">
         <v>62</v>
@@ -3875,13 +3887,13 @@
         <v>101</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P43">
         <v>100</v>
       </c>
       <c r="Q43" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3912,10 +3924,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J44" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="K44" t="s">
         <v>62</v>
@@ -3930,13 +3942,13 @@
         <v>101</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="P44">
         <v>100</v>
       </c>
       <c r="Q44" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3967,7 +3979,7 @@
         <v>1683</v>
       </c>
       <c r="I45" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J45" t="s">
         <v>6</v>
@@ -3985,13 +3997,13 @@
         <v>6</v>
       </c>
       <c r="O45" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P45">
         <v>100</v>
       </c>
       <c r="Q45" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -4022,7 +4034,7 @@
         <v>1806</v>
       </c>
       <c r="I46" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J46" t="s">
         <v>6</v>
@@ -4040,13 +4052,13 @@
         <v>6</v>
       </c>
       <c r="O46" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P46">
         <v>100</v>
       </c>
       <c r="Q46" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -4077,7 +4089,7 @@
         <v>1801</v>
       </c>
       <c r="I47" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J47" t="s">
         <v>6</v>
@@ -4095,13 +4107,13 @@
         <v>6</v>
       </c>
       <c r="O47" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P47">
         <v>100</v>
       </c>
       <c r="Q47" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -4132,7 +4144,7 @@
         <v>1794</v>
       </c>
       <c r="I48" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J48" t="s">
         <v>6</v>
@@ -4150,13 +4162,13 @@
         <v>6</v>
       </c>
       <c r="O48" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P48">
         <v>100</v>
       </c>
       <c r="Q48" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -4187,7 +4199,7 @@
         <v>1789</v>
       </c>
       <c r="I49" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J49" t="s">
         <v>6</v>
@@ -4205,13 +4217,13 @@
         <v>6</v>
       </c>
       <c r="O49" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P49">
         <v>100</v>
       </c>
       <c r="Q49" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -4242,7 +4254,7 @@
         <v>1789</v>
       </c>
       <c r="I50" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J50" t="s">
         <v>6</v>
@@ -4260,13 +4272,13 @@
         <v>6</v>
       </c>
       <c r="O50" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P50">
         <v>100</v>
       </c>
       <c r="Q50" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -4297,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J51" t="s">
         <v>6</v>
@@ -4315,13 +4327,13 @@
         <v>6</v>
       </c>
       <c r="O51" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P51">
         <v>100</v>
       </c>
       <c r="Q51" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -4352,7 +4364,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J52" t="s">
         <v>6</v>
@@ -4370,13 +4382,13 @@
         <v>6</v>
       </c>
       <c r="O52" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P52">
         <v>100</v>
       </c>
       <c r="Q52" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -4407,7 +4419,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J53" t="s">
         <v>6</v>
@@ -4425,13 +4437,13 @@
         <v>6</v>
       </c>
       <c r="O53" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P53">
         <v>100</v>
       </c>
       <c r="Q53" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -4462,7 +4474,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J54" t="s">
         <v>6</v>
@@ -4480,13 +4492,13 @@
         <v>6</v>
       </c>
       <c r="O54" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P54">
         <v>100</v>
       </c>
       <c r="Q54" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -4517,7 +4529,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J55" t="s">
         <v>6</v>
@@ -4535,13 +4547,13 @@
         <v>6</v>
       </c>
       <c r="O55" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P55">
         <v>100</v>
       </c>
       <c r="Q55" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -4572,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J56" t="s">
         <v>6</v>
@@ -4590,13 +4602,13 @@
         <v>6</v>
       </c>
       <c r="O56" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P56">
         <v>100</v>
       </c>
       <c r="Q56" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -4627,7 +4639,7 @@
         <v>1709</v>
       </c>
       <c r="I57" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J57" t="s">
         <v>6</v>
@@ -4645,13 +4657,13 @@
         <v>6</v>
       </c>
       <c r="O57" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P57">
         <v>100</v>
       </c>
       <c r="Q57" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -4682,7 +4694,7 @@
         <v>1704</v>
       </c>
       <c r="I58" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J58" t="s">
         <v>6</v>
@@ -4700,13 +4712,13 @@
         <v>6</v>
       </c>
       <c r="O58" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P58">
         <v>100</v>
       </c>
       <c r="Q58" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -4737,7 +4749,7 @@
         <v>1898</v>
       </c>
       <c r="I59" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J59" t="s">
         <v>6</v>
@@ -4755,13 +4767,13 @@
         <v>6</v>
       </c>
       <c r="O59" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P59">
         <v>100</v>
       </c>
       <c r="Q59" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -4792,7 +4804,7 @@
         <v>1887</v>
       </c>
       <c r="I60" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J60" t="s">
         <v>6</v>
@@ -4810,13 +4822,13 @@
         <v>6</v>
       </c>
       <c r="O60" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P60">
         <v>100</v>
       </c>
       <c r="Q60" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -4847,7 +4859,7 @@
         <v>1964</v>
       </c>
       <c r="I61" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J61" t="s">
         <v>6</v>
@@ -4865,13 +4877,13 @@
         <v>6</v>
       </c>
       <c r="O61" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P61">
         <v>100</v>
       </c>
       <c r="Q61" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -4902,7 +4914,7 @@
         <v>1866</v>
       </c>
       <c r="I62" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J62" t="s">
         <v>6</v>
@@ -4920,13 +4932,13 @@
         <v>6</v>
       </c>
       <c r="O62" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P62">
         <v>100</v>
       </c>
       <c r="Q62" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -4957,7 +4969,7 @@
         <v>1863</v>
       </c>
       <c r="I63" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J63" t="s">
         <v>6</v>
@@ -4975,13 +4987,13 @@
         <v>6</v>
       </c>
       <c r="O63" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P63">
         <v>100</v>
       </c>
       <c r="Q63" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -5012,7 +5024,7 @@
         <v>1860</v>
       </c>
       <c r="I64" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J64" t="s">
         <v>6</v>
@@ -5030,13 +5042,13 @@
         <v>6</v>
       </c>
       <c r="O64" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P64">
         <v>100</v>
       </c>
       <c r="Q64" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -5067,7 +5079,7 @@
         <v>1788</v>
       </c>
       <c r="I65" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J65" t="s">
         <v>6</v>
@@ -5085,13 +5097,13 @@
         <v>6</v>
       </c>
       <c r="O65" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P65">
         <v>100</v>
       </c>
       <c r="Q65" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:17">
@@ -5122,7 +5134,7 @@
         <v>1786</v>
       </c>
       <c r="I66" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J66" t="s">
         <v>6</v>
@@ -5140,13 +5152,13 @@
         <v>6</v>
       </c>
       <c r="O66" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P66">
         <v>100</v>
       </c>
       <c r="Q66" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -5177,7 +5189,7 @@
         <v>1766</v>
       </c>
       <c r="I67" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="J67" t="s">
         <v>6</v>
@@ -5195,13 +5207,13 @@
         <v>6</v>
       </c>
       <c r="O67" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P67">
         <v>100</v>
       </c>
       <c r="Q67" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -5232,7 +5244,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J68" t="s">
         <v>6</v>
@@ -5250,13 +5262,13 @@
         <v>6</v>
       </c>
       <c r="O68" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P68">
         <v>100</v>
       </c>
-      <c r="Q68" s="9" t="s">
-        <v>209</v>
+      <c r="Q68" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -5287,7 +5299,7 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J69" t="s">
         <v>6</v>
@@ -5305,13 +5317,13 @@
         <v>6</v>
       </c>
       <c r="O69" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P69">
         <v>100</v>
       </c>
-      <c r="Q69" t="s">
-        <v>210</v>
+      <c r="Q69" s="9" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -5342,7 +5354,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="J70" t="s">
         <v>6</v>
@@ -5360,13 +5372,13 @@
         <v>6</v>
       </c>
       <c r="O70" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="P70">
         <v>100</v>
       </c>
       <c r="Q70" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>